<commit_message>
complete with plot 2
</commit_message>
<xml_diff>
--- a/prediction_with_lag/output/dollar.xlsx
+++ b/prediction_with_lag/output/dollar.xlsx
@@ -461,10 +461,10 @@
         <v>45427</v>
       </c>
       <c r="B2" t="n">
-        <v>587127</v>
+        <v>592091</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01331980898976326</v>
+        <v>-0.004900305531919003</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>45428</v>
       </c>
       <c r="B3" t="n">
-        <v>594617</v>
+        <v>587032</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01267711073160172</v>
+        <v>-0.008581390604376793</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         <v>45429</v>
       </c>
       <c r="B4" t="n">
-        <v>593436</v>
+        <v>594678</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.001987839350476861</v>
+        <v>0.01294092461466789</v>
       </c>
     </row>
     <row r="5">
@@ -494,10 +494,10 @@
         <v>45430</v>
       </c>
       <c r="B5" t="n">
-        <v>602610</v>
+        <v>622732</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0153403403237462</v>
+        <v>0.04609593376517296</v>
       </c>
     </row>
     <row r="6">
@@ -505,10 +505,10 @@
         <v>45431</v>
       </c>
       <c r="B6" t="n">
-        <v>605493</v>
+        <v>636010</v>
       </c>
       <c r="C6" t="n">
-        <v>0.004772607702761889</v>
+        <v>0.02109854109585285</v>
       </c>
     </row>
     <row r="7">
@@ -516,10 +516,10 @@
         <v>45432</v>
       </c>
       <c r="B7" t="n">
-        <v>611569</v>
+        <v>634981</v>
       </c>
       <c r="C7" t="n">
-        <v>0.009984842501580715</v>
+        <v>-0.001619063667021692</v>
       </c>
     </row>
     <row r="8">
@@ -527,10 +527,10 @@
         <v>45433</v>
       </c>
       <c r="B8" t="n">
-        <v>614215</v>
+        <v>629714</v>
       </c>
       <c r="C8" t="n">
-        <v>0.004316866397857666</v>
+        <v>-0.008328898809850216</v>
       </c>
     </row>
     <row r="9">
@@ -538,10 +538,10 @@
         <v>45434</v>
       </c>
       <c r="B9" t="n">
-        <v>618587</v>
+        <v>627068</v>
       </c>
       <c r="C9" t="n">
-        <v>0.007093477994203568</v>
+        <v>-0.004210436251014471</v>
       </c>
     </row>
     <row r="10">
@@ -549,10 +549,10 @@
         <v>45435</v>
       </c>
       <c r="B10" t="n">
-        <v>621775</v>
+        <v>631229</v>
       </c>
       <c r="C10" t="n">
-        <v>0.005140581168234348</v>
+        <v>0.00661390321329236</v>
       </c>
     </row>
     <row r="11">
@@ -560,10 +560,10 @@
         <v>45436</v>
       </c>
       <c r="B11" t="n">
-        <v>642010</v>
+        <v>633555</v>
       </c>
       <c r="C11" t="n">
-        <v>0.03202566877007484</v>
+        <v>0.003678879700601101</v>
       </c>
     </row>
     <row r="12">
@@ -571,10 +571,10 @@
         <v>45437</v>
       </c>
       <c r="B12" t="n">
-        <v>643861</v>
+        <v>632502</v>
       </c>
       <c r="C12" t="n">
-        <v>0.002879413077607751</v>
+        <v>-0.001662912545725703</v>
       </c>
     </row>
     <row r="13">
@@ -582,10 +582,10 @@
         <v>45438</v>
       </c>
       <c r="B13" t="n">
-        <v>647565</v>
+        <v>627845</v>
       </c>
       <c r="C13" t="n">
-        <v>0.005736578721553087</v>
+        <v>-0.007390342652797699</v>
       </c>
     </row>
     <row r="14">
@@ -593,10 +593,10 @@
         <v>45439</v>
       </c>
       <c r="B14" t="n">
-        <v>651059</v>
+        <v>626907</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00538169126957655</v>
+        <v>-0.001495314529165626</v>
       </c>
     </row>
     <row r="15">
@@ -604,10 +604,10 @@
         <v>45440</v>
       </c>
       <c r="B15" t="n">
-        <v>677402</v>
+        <v>625399</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03966455161571503</v>
+        <v>-0.002408578991889954</v>
       </c>
     </row>
     <row r="16">
@@ -615,10 +615,10 @@
         <v>45441</v>
       </c>
       <c r="B16" t="n">
-        <v>669648</v>
+        <v>627828</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.0115124611184001</v>
+        <v>0.003876081435009837</v>
       </c>
     </row>
     <row r="17">
@@ -626,10 +626,10 @@
         <v>45442</v>
       </c>
       <c r="B17" t="n">
-        <v>661047</v>
+        <v>630155</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.01292662601917982</v>
+        <v>0.003700263798236847</v>
       </c>
     </row>
     <row r="18">
@@ -637,10 +637,10 @@
         <v>45443</v>
       </c>
       <c r="B18" t="n">
-        <v>648946</v>
+        <v>632391</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.01847472414374352</v>
+        <v>0.003541411831974983</v>
       </c>
     </row>
     <row r="19">
@@ -648,10 +648,10 @@
         <v>45444</v>
       </c>
       <c r="B19" t="n">
-        <v>643681</v>
+        <v>634004</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.008145714178681374</v>
+        <v>0.002547688782215118</v>
       </c>
     </row>
     <row r="20">
@@ -659,10 +659,10 @@
         <v>45445</v>
       </c>
       <c r="B20" t="n">
-        <v>639609</v>
+        <v>634045</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.006346569862216711</v>
+        <v>6.418088742066175e-05</v>
       </c>
     </row>
     <row r="21">
@@ -670,10 +670,10 @@
         <v>45446</v>
       </c>
       <c r="B21" t="n">
-        <v>624526</v>
+        <v>638199</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.02386431396007538</v>
+        <v>0.006530053913593292</v>
       </c>
     </row>
     <row r="22">
@@ -681,10 +681,10 @@
         <v>45447</v>
       </c>
       <c r="B22" t="n">
-        <v>621708</v>
+        <v>637741</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.004522307310253382</v>
+        <v>-0.0007174259517341852</v>
       </c>
     </row>
     <row r="23">
@@ -692,10 +692,10 @@
         <v>45448</v>
       </c>
       <c r="B23" t="n">
-        <v>622337</v>
+        <v>629357</v>
       </c>
       <c r="C23" t="n">
-        <v>0.00101159792393446</v>
+        <v>-0.01323303300887346</v>
       </c>
     </row>
     <row r="24">
@@ -703,10 +703,10 @@
         <v>45449</v>
       </c>
       <c r="B24" t="n">
-        <v>625755</v>
+        <v>631768</v>
       </c>
       <c r="C24" t="n">
-        <v>0.005476986058056355</v>
+        <v>0.003823841223493218</v>
       </c>
     </row>
     <row r="25">
@@ -714,10 +714,10 @@
         <v>45450</v>
       </c>
       <c r="B25" t="n">
-        <v>623452</v>
+        <v>629879</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.00368717685341835</v>
+        <v>-0.002994842361658812</v>
       </c>
     </row>
     <row r="26">
@@ -725,10 +725,10 @@
         <v>45451</v>
       </c>
       <c r="B26" t="n">
-        <v>621744</v>
+        <v>633204</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.002743382006883621</v>
+        <v>0.005265426822006702</v>
       </c>
     </row>
     <row r="27">
@@ -736,10 +736,10 @@
         <v>45452</v>
       </c>
       <c r="B27" t="n">
-        <v>627162</v>
+        <v>637285</v>
       </c>
       <c r="C27" t="n">
-        <v>0.008675825782120228</v>
+        <v>0.006425098981708288</v>
       </c>
     </row>
     <row r="28">
@@ -747,10 +747,10 @@
         <v>45453</v>
       </c>
       <c r="B28" t="n">
-        <v>631974</v>
+        <v>633987</v>
       </c>
       <c r="C28" t="n">
-        <v>0.007644115015864372</v>
+        <v>-0.005188418086618185</v>
       </c>
     </row>
     <row r="29">
@@ -758,10 +758,10 @@
         <v>45454</v>
       </c>
       <c r="B29" t="n">
-        <v>626600</v>
+        <v>631765</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.00854051485657692</v>
+        <v>-0.003510715439915657</v>
       </c>
     </row>
     <row r="30">
@@ -769,10 +769,10 @@
         <v>45455</v>
       </c>
       <c r="B30" t="n">
-        <v>629451</v>
+        <v>630361</v>
       </c>
       <c r="C30" t="n">
-        <v>0.004540124908089638</v>
+        <v>-0.002224794821813703</v>
       </c>
     </row>
     <row r="31">
@@ -780,10 +780,10 @@
         <v>45456</v>
       </c>
       <c r="B31" t="n">
-        <v>633377</v>
+        <v>634017</v>
       </c>
       <c r="C31" t="n">
-        <v>0.006218590773642063</v>
+        <v>0.00578342517837882</v>
       </c>
     </row>
     <row r="32">
@@ -791,10 +791,10 @@
         <v>45457</v>
       </c>
       <c r="B32" t="n">
-        <v>646415</v>
+        <v>633177</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0203761663287878</v>
+        <v>-0.001326139783486724</v>
       </c>
     </row>
     <row r="33">
@@ -802,10 +802,10 @@
         <v>45458</v>
       </c>
       <c r="B33" t="n">
-        <v>636572</v>
+        <v>625531</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.01534464117139578</v>
+        <v>-0.01214920729398727</v>
       </c>
     </row>
     <row r="34">
@@ -813,10 +813,10 @@
         <v>45459</v>
       </c>
       <c r="B34" t="n">
-        <v>637022</v>
+        <v>622915</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0007059239433147013</v>
+        <v>-0.004191330634057522</v>
       </c>
     </row>
     <row r="35">
@@ -824,10 +824,10 @@
         <v>45460</v>
       </c>
       <c r="B35" t="n">
-        <v>641263</v>
+        <v>625226</v>
       </c>
       <c r="C35" t="n">
-        <v>0.00663501163944602</v>
+        <v>0.003702787915244699</v>
       </c>
     </row>
     <row r="36">
@@ -835,10 +835,10 @@
         <v>45461</v>
       </c>
       <c r="B36" t="n">
-        <v>643048</v>
+        <v>630674</v>
       </c>
       <c r="C36" t="n">
-        <v>0.002778941299766302</v>
+        <v>0.008675815537571907</v>
       </c>
     </row>
     <row r="37">
@@ -846,10 +846,10 @@
         <v>45462</v>
       </c>
       <c r="B37" t="n">
-        <v>638036</v>
+        <v>631872</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.007824094034731388</v>
+        <v>0.001898121903650463</v>
       </c>
     </row>
     <row r="38">
@@ -857,10 +857,10 @@
         <v>45463</v>
       </c>
       <c r="B38" t="n">
-        <v>639713</v>
+        <v>627885</v>
       </c>
       <c r="C38" t="n">
-        <v>0.002624543616548181</v>
+        <v>-0.006329057272523642</v>
       </c>
     </row>
     <row r="39">
@@ -868,10 +868,10 @@
         <v>45464</v>
       </c>
       <c r="B39" t="n">
-        <v>644975</v>
+        <v>631581</v>
       </c>
       <c r="C39" t="n">
-        <v>0.008191307075321674</v>
+        <v>0.005869032815098763</v>
       </c>
     </row>
     <row r="40">
@@ -879,10 +879,10 @@
         <v>45465</v>
       </c>
       <c r="B40" t="n">
-        <v>657091</v>
+        <v>635209</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01861025579273701</v>
+        <v>0.005727432668209076</v>
       </c>
     </row>
     <row r="41">
@@ -890,10 +890,10 @@
         <v>45466</v>
       </c>
       <c r="B41" t="n">
-        <v>653772</v>
+        <v>629330</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.005063422024250031</v>
+        <v>-0.009297622367739677</v>
       </c>
     </row>
     <row r="42">
@@ -901,10 +901,10 @@
         <v>45467</v>
       </c>
       <c r="B42" t="n">
-        <v>654791</v>
+        <v>627493</v>
       </c>
       <c r="C42" t="n">
-        <v>0.001557437353767455</v>
+        <v>-0.00292280176654458</v>
       </c>
     </row>
     <row r="43">
@@ -912,10 +912,10 @@
         <v>45468</v>
       </c>
       <c r="B43" t="n">
-        <v>666332</v>
+        <v>629883</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01747238449752331</v>
+        <v>0.003801406361162663</v>
       </c>
     </row>
     <row r="44">
@@ -923,10 +923,10 @@
         <v>45469</v>
       </c>
       <c r="B44" t="n">
-        <v>670826</v>
+        <v>632861</v>
       </c>
       <c r="C44" t="n">
-        <v>0.006721506360918283</v>
+        <v>0.004716643132269382</v>
       </c>
     </row>
     <row r="45">
@@ -934,10 +934,10 @@
         <v>45470</v>
       </c>
       <c r="B45" t="n">
-        <v>684670</v>
+        <v>628497</v>
       </c>
       <c r="C45" t="n">
-        <v>0.02042657695710659</v>
+        <v>-0.006918886676430702</v>
       </c>
     </row>
     <row r="46">
@@ -945,10 +945,10 @@
         <v>45471</v>
       </c>
       <c r="B46" t="n">
-        <v>680455</v>
+        <v>629485</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.006174721289426088</v>
+        <v>0.001571498229168355</v>
       </c>
     </row>
     <row r="47">
@@ -956,10 +956,10 @@
         <v>45472</v>
       </c>
       <c r="B47" t="n">
-        <v>677700</v>
+        <v>622664</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.004057156853377819</v>
+        <v>-0.01089569460600615</v>
       </c>
     </row>
     <row r="48">
@@ -967,10 +967,10 @@
         <v>45473</v>
       </c>
       <c r="B48" t="n">
-        <v>678365</v>
+        <v>627286</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0009810016490519047</v>
+        <v>0.00739624397829175</v>
       </c>
     </row>
     <row r="49">
@@ -978,10 +978,10 @@
         <v>45474</v>
       </c>
       <c r="B49" t="n">
-        <v>677815</v>
+        <v>623812</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.0008116330136545002</v>
+        <v>-0.005552992690354586</v>
       </c>
     </row>
     <row r="50">
@@ -989,10 +989,10 @@
         <v>45475</v>
       </c>
       <c r="B50" t="n">
-        <v>676145</v>
+        <v>625022</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.002466409932821989</v>
+        <v>0.001938386703841388</v>
       </c>
     </row>
     <row r="51">
@@ -1000,10 +1000,10 @@
         <v>45476</v>
       </c>
       <c r="B51" t="n">
-        <v>671294</v>
+        <v>619836</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.00720047065988183</v>
+        <v>-0.008332218043506145</v>
       </c>
     </row>
     <row r="52">
@@ -1011,10 +1011,10 @@
         <v>45477</v>
       </c>
       <c r="B52" t="n">
-        <v>670984</v>
+        <v>620964</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.0004617282247636467</v>
+        <v>0.001818535034544766</v>
       </c>
     </row>
     <row r="53">
@@ -1022,10 +1022,10 @@
         <v>45478</v>
       </c>
       <c r="B53" t="n">
-        <v>670992</v>
+        <v>615622</v>
       </c>
       <c r="C53" t="n">
-        <v>1.225891355716158e-05</v>
+        <v>-0.008640664629638195</v>
       </c>
     </row>
     <row r="54">
@@ -1033,10 +1033,10 @@
         <v>45479</v>
       </c>
       <c r="B54" t="n">
-        <v>673420</v>
+        <v>610330</v>
       </c>
       <c r="C54" t="n">
-        <v>0.003611858235672116</v>
+        <v>-0.008633963763713837</v>
       </c>
     </row>
     <row r="55">
@@ -1044,10 +1044,10 @@
         <v>45480</v>
       </c>
       <c r="B55" t="n">
-        <v>674165</v>
+        <v>610323</v>
       </c>
       <c r="C55" t="n">
-        <v>0.001104997936636209</v>
+        <v>-1.112596783059416e-05</v>
       </c>
     </row>
     <row r="56">
@@ -1055,10 +1055,10 @@
         <v>45481</v>
       </c>
       <c r="B56" t="n">
-        <v>672584</v>
+        <v>609382</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.002348289825022221</v>
+        <v>-0.001542193465866148</v>
       </c>
     </row>
     <row r="57">
@@ -1066,10 +1066,10 @@
         <v>45482</v>
       </c>
       <c r="B57" t="n">
-        <v>674267</v>
+        <v>613031</v>
       </c>
       <c r="C57" t="n">
-        <v>0.002498806454241276</v>
+        <v>0.005970211233943701</v>
       </c>
     </row>
     <row r="58">
@@ -1077,10 +1077,10 @@
         <v>45483</v>
       </c>
       <c r="B58" t="n">
-        <v>679051</v>
+        <v>614824</v>
       </c>
       <c r="C58" t="n">
-        <v>0.007069436833262444</v>
+        <v>0.002919837366789579</v>
       </c>
     </row>
     <row r="59">
@@ -1088,10 +1088,10 @@
         <v>45484</v>
       </c>
       <c r="B59" t="n">
-        <v>678395</v>
+        <v>615854</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.0009669006685726345</v>
+        <v>0.001674434752203524</v>
       </c>
     </row>
     <row r="60">
@@ -1099,10 +1099,10 @@
         <v>45485</v>
       </c>
       <c r="B60" t="n">
-        <v>678660</v>
+        <v>615721</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0003912048996426165</v>
+        <v>-0.000215426945942454</v>
       </c>
     </row>
     <row r="61">
@@ -1110,10 +1110,10 @@
         <v>45486</v>
       </c>
       <c r="B61" t="n">
-        <v>684376</v>
+        <v>615426</v>
       </c>
       <c r="C61" t="n">
-        <v>0.008386557921767235</v>
+        <v>-0.0004790779494214803</v>
       </c>
     </row>
     <row r="62">
@@ -1121,10 +1121,10 @@
         <v>45487</v>
       </c>
       <c r="B62" t="n">
-        <v>686734</v>
+        <v>618288</v>
       </c>
       <c r="C62" t="n">
-        <v>0.00344009161926806</v>
+        <v>0.004640447907149792</v>
       </c>
     </row>
     <row r="63">
@@ -1132,10 +1132,10 @@
         <v>45488</v>
       </c>
       <c r="B63" t="n">
-        <v>687542</v>
+        <v>619164</v>
       </c>
       <c r="C63" t="n">
-        <v>0.001176198711618781</v>
+        <v>0.001415095292031765</v>
       </c>
     </row>
     <row r="64">
@@ -1143,10 +1143,10 @@
         <v>45489</v>
       </c>
       <c r="B64" t="n">
-        <v>693185</v>
+        <v>620238</v>
       </c>
       <c r="C64" t="n">
-        <v>0.008174438029527664</v>
+        <v>0.001733743702061474</v>
       </c>
     </row>
     <row r="65">
@@ -1154,10 +1154,10 @@
         <v>45490</v>
       </c>
       <c r="B65" t="n">
-        <v>697200</v>
+        <v>617556</v>
       </c>
       <c r="C65" t="n">
-        <v>0.005774713587015867</v>
+        <v>-0.004333783406764269</v>
       </c>
     </row>
     <row r="66">
@@ -1165,10 +1165,10 @@
         <v>45491</v>
       </c>
       <c r="B66" t="n">
-        <v>700419</v>
+        <v>617939</v>
       </c>
       <c r="C66" t="n">
-        <v>0.004606105852872133</v>
+        <v>0.0006206942489370704</v>
       </c>
     </row>
     <row r="67">
@@ -1176,10 +1176,10 @@
         <v>45492</v>
       </c>
       <c r="B67" t="n">
-        <v>704325</v>
+        <v>620760</v>
       </c>
       <c r="C67" t="n">
-        <v>0.005560793448239565</v>
+        <v>0.004555430728942156</v>
       </c>
     </row>
     <row r="68">
@@ -1187,10 +1187,10 @@
         <v>45493</v>
       </c>
       <c r="B68" t="n">
-        <v>707862</v>
+        <v>620569</v>
       </c>
       <c r="C68" t="n">
-        <v>0.005009056068956852</v>
+        <v>-0.0003071909595746547</v>
       </c>
     </row>
     <row r="69">
@@ -1198,10 +1198,10 @@
         <v>45494</v>
       </c>
       <c r="B69" t="n">
-        <v>731891</v>
+        <v>615955</v>
       </c>
       <c r="C69" t="n">
-        <v>0.033382598310709</v>
+        <v>-0.007462609559297562</v>
       </c>
     </row>
     <row r="70">
@@ -1209,10 +1209,10 @@
         <v>45495</v>
       </c>
       <c r="B70" t="n">
-        <v>735488</v>
+        <v>616727</v>
       </c>
       <c r="C70" t="n">
-        <v>0.004902416374534369</v>
+        <v>0.001253113965503871</v>
       </c>
     </row>
     <row r="71">
@@ -1220,10 +1220,10 @@
         <v>45496</v>
       </c>
       <c r="B71" t="n">
-        <v>759206</v>
+        <v>619192</v>
       </c>
       <c r="C71" t="n">
-        <v>0.03173937276005745</v>
+        <v>0.003989258781075478</v>
       </c>
     </row>
     <row r="72">
@@ -1231,10 +1231,10 @@
         <v>45497</v>
       </c>
       <c r="B72" t="n">
-        <v>734088</v>
+        <v>619961</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.03364363685250282</v>
+        <v>0.001241911319084466</v>
       </c>
     </row>
     <row r="73">
@@ -1242,10 +1242,10 @@
         <v>45498</v>
       </c>
       <c r="B73" t="n">
-        <v>755831</v>
+        <v>620987</v>
       </c>
       <c r="C73" t="n">
-        <v>0.02918888069689274</v>
+        <v>0.001653402228839695</v>
       </c>
     </row>
     <row r="74">
@@ -1253,10 +1253,10 @@
         <v>45499</v>
       </c>
       <c r="B74" t="n">
-        <v>747874</v>
+        <v>622089</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.01058332528918982</v>
+        <v>0.001773793832398951</v>
       </c>
     </row>
     <row r="75">
@@ -1264,10 +1264,10 @@
         <v>45500</v>
       </c>
       <c r="B75" t="n">
-        <v>751892</v>
+        <v>621679</v>
       </c>
       <c r="C75" t="n">
-        <v>0.00535808177664876</v>
+        <v>-0.0006596596795134246</v>
       </c>
     </row>
     <row r="76">
@@ -1275,10 +1275,10 @@
         <v>45501</v>
       </c>
       <c r="B76" t="n">
-        <v>754327</v>
+        <v>620120</v>
       </c>
       <c r="C76" t="n">
-        <v>0.00323301856406033</v>
+        <v>-0.002511280123144388</v>
       </c>
     </row>
     <row r="77">
@@ -1286,10 +1286,10 @@
         <v>45502</v>
       </c>
       <c r="B77" t="n">
-        <v>757761</v>
+        <v>621691</v>
       </c>
       <c r="C77" t="n">
-        <v>0.004541587550193071</v>
+        <v>0.002529565012082458</v>
       </c>
     </row>
     <row r="78">
@@ -1297,10 +1297,10 @@
         <v>45503</v>
       </c>
       <c r="B78" t="n">
-        <v>748223</v>
+        <v>621806</v>
       </c>
       <c r="C78" t="n">
-        <v>-0.01266681123524904</v>
+        <v>0.0001856459712143987</v>
       </c>
     </row>
     <row r="79">
@@ -1308,10 +1308,10 @@
         <v>45504</v>
       </c>
       <c r="B79" t="n">
-        <v>741253</v>
+        <v>625149</v>
       </c>
       <c r="C79" t="n">
-        <v>-0.009358800947666168</v>
+        <v>0.005361692514270544</v>
       </c>
     </row>
     <row r="80">
@@ -1319,10 +1319,10 @@
         <v>45505</v>
       </c>
       <c r="B80" t="n">
-        <v>736377</v>
+        <v>622988</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.00659960089251399</v>
+        <v>-0.003462595632299781</v>
       </c>
     </row>
     <row r="81">
@@ -1330,10 +1330,10 @@
         <v>45506</v>
       </c>
       <c r="B81" t="n">
-        <v>737329</v>
+        <v>622560</v>
       </c>
       <c r="C81" t="n">
-        <v>0.001291819266043603</v>
+        <v>-0.0006872529629617929</v>
       </c>
     </row>
     <row r="82">
@@ -1341,10 +1341,10 @@
         <v>45507</v>
       </c>
       <c r="B82" t="n">
-        <v>734209</v>
+        <v>626333</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.004240469541400671</v>
+        <v>0.0060426932759583</v>
       </c>
     </row>
     <row r="83">
@@ -1352,10 +1352,10 @@
         <v>45508</v>
       </c>
       <c r="B83" t="n">
-        <v>730792</v>
+        <v>625523</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.004665367305278778</v>
+        <v>-0.001293898443691432</v>
       </c>
     </row>
     <row r="84">
@@ -1363,10 +1363,10 @@
         <v>45509</v>
       </c>
       <c r="B84" t="n">
-        <v>729197</v>
+        <v>623546</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.002184724435210228</v>
+        <v>-0.003165753558278084</v>
       </c>
     </row>
     <row r="85">
@@ -1374,10 +1374,10 @@
         <v>45510</v>
       </c>
       <c r="B85" t="n">
-        <v>723601</v>
+        <v>622265</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.007704097311943769</v>
+        <v>-0.002056481316685677</v>
       </c>
     </row>
     <row r="86">
@@ -1385,10 +1385,10 @@
         <v>45511</v>
       </c>
       <c r="B86" t="n">
-        <v>724168</v>
+        <v>625856</v>
       </c>
       <c r="C86" t="n">
-        <v>0.0007836771546863019</v>
+        <v>0.005753915291279554</v>
       </c>
     </row>
     <row r="87">
@@ -1396,10 +1396,10 @@
         <v>45512</v>
       </c>
       <c r="B87" t="n">
-        <v>724619</v>
+        <v>627232</v>
       </c>
       <c r="C87" t="n">
-        <v>0.0006225354736670852</v>
+        <v>0.002196959452703595</v>
       </c>
     </row>
     <row r="88">
@@ -1407,10 +1407,10 @@
         <v>45513</v>
       </c>
       <c r="B88" t="n">
-        <v>725132</v>
+        <v>625665</v>
       </c>
       <c r="C88" t="n">
-        <v>0.0007081158109940588</v>
+        <v>-0.002501975512132049</v>
       </c>
     </row>
     <row r="89">
@@ -1418,10 +1418,10 @@
         <v>45514</v>
       </c>
       <c r="B89" t="n">
-        <v>724769</v>
+        <v>628317</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.0005010789027437568</v>
+        <v>0.004230115562677383</v>
       </c>
     </row>
     <row r="90">
@@ -1429,10 +1429,10 @@
         <v>45515</v>
       </c>
       <c r="B90" t="n">
-        <v>727132</v>
+        <v>627718</v>
       </c>
       <c r="C90" t="n">
-        <v>0.003254613373428583</v>
+        <v>-0.0009538685553707182</v>
       </c>
     </row>
     <row r="91">
@@ -1440,10 +1440,10 @@
         <v>45516</v>
       </c>
       <c r="B91" t="n">
-        <v>733106</v>
+        <v>608960</v>
       </c>
       <c r="C91" t="n">
-        <v>0.008182878606021404</v>
+        <v>-0.03033816628158092</v>
       </c>
     </row>
     <row r="92">
@@ -1451,10 +1451,10 @@
         <v>45517</v>
       </c>
       <c r="B92" t="n">
-        <v>732951</v>
+        <v>610203</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.0002110061468556523</v>
+        <v>0.002039549173787236</v>
       </c>
     </row>
     <row r="93">
@@ -1462,10 +1462,10 @@
         <v>45518</v>
       </c>
       <c r="B93" t="n">
-        <v>735867</v>
+        <v>609414</v>
       </c>
       <c r="C93" t="n">
-        <v>0.003970160614699125</v>
+        <v>-0.001293927896767855</v>
       </c>
     </row>
     <row r="94">
@@ -1473,10 +1473,10 @@
         <v>45519</v>
       </c>
       <c r="B94" t="n">
-        <v>743115</v>
+        <v>609430</v>
       </c>
       <c r="C94" t="n">
-        <v>0.009801439940929413</v>
+        <v>2.577547638793476e-05</v>
       </c>
     </row>
     <row r="95">
@@ -1484,10 +1484,10 @@
         <v>45520</v>
       </c>
       <c r="B95" t="n">
-        <v>752485</v>
+        <v>613690</v>
       </c>
       <c r="C95" t="n">
-        <v>0.01252966374158859</v>
+        <v>0.006965355481952429</v>
       </c>
     </row>
     <row r="96">
@@ -1495,10 +1495,10 @@
         <v>45521</v>
       </c>
       <c r="B96" t="n">
-        <v>755038</v>
+        <v>609774</v>
       </c>
       <c r="C96" t="n">
-        <v>0.003387531032785773</v>
+        <v>-0.006401112768799067</v>
       </c>
     </row>
     <row r="97">
@@ -1506,10 +1506,10 @@
         <v>45522</v>
       </c>
       <c r="B97" t="n">
-        <v>761986</v>
+        <v>608980</v>
       </c>
       <c r="C97" t="n">
-        <v>0.009160353802144527</v>
+        <v>-0.001303470693528652</v>
       </c>
     </row>
     <row r="98">
@@ -1517,10 +1517,10 @@
         <v>45523</v>
       </c>
       <c r="B98" t="n">
-        <v>771560</v>
+        <v>612687</v>
       </c>
       <c r="C98" t="n">
-        <v>0.01248570997267962</v>
+        <v>0.006069098133593798</v>
       </c>
     </row>
     <row r="99">
@@ -1528,10 +1528,10 @@
         <v>45524</v>
       </c>
       <c r="B99" t="n">
-        <v>776953</v>
+        <v>615352</v>
       </c>
       <c r="C99" t="n">
-        <v>0.006965445354580879</v>
+        <v>0.004339731764048338</v>
       </c>
     </row>
     <row r="100">
@@ -1539,10 +1539,10 @@
         <v>45525</v>
       </c>
       <c r="B100" t="n">
-        <v>797063</v>
+        <v>609257</v>
       </c>
       <c r="C100" t="n">
-        <v>0.02555330842733383</v>
+        <v>-0.009954815730452538</v>
       </c>
     </row>
     <row r="101">
@@ -1550,10 +1550,10 @@
         <v>45526</v>
       </c>
       <c r="B101" t="n">
-        <v>786432</v>
+        <v>607702</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.0134273050352931</v>
+        <v>-0.002555917017161846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>